<commit_message>
u*/ws analysis for all SS sizes un suspension
- got a SS record for all sizes
- tried calibrating Cm to lower tau mobile, but idk if it worked or not or if elowyn likes it?
</commit_message>
<xml_diff>
--- a/Shear Stress/shear_velocity/settling_velocity_calculation.xlsx
+++ b/Shear Stress/shear_velocity/settling_velocity_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Shear Stress\shear_velocity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE5AF94-AF4A-47F2-99F2-083F9E6782AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04CF2DF-E512-49F5-98A3-762F5E3D7898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t xml:space="preserve">Dn </t>
   </si>
@@ -172,6 +172,9 @@
   <si>
     <t>Coarse Sand</t>
   </si>
+  <si>
+    <t>Size</t>
+  </si>
 </sst>
 </file>
 
@@ -181,7 +184,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -368,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -553,23 +556,50 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -583,14 +613,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -598,78 +628,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5967,10 +5936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z53"/>
+  <dimension ref="A1:AA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5983,7 +5952,7 @@
     <col min="25" max="25" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -6009,18 +5978,18 @@
       <c r="I1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="71" t="s">
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
       <c r="R1" s="16" t="s">
         <v>21</v>
       </c>
@@ -6040,7 +6009,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -6108,8 +6077,11 @@
       <c r="Y2" s="21" t="s">
         <v>38</v>
       </c>
+      <c r="AA2" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -6188,7 +6160,7 @@
         <f>((S3*($C$3-$C$9)*$C$4*$C$11)/$C$9)^(1/3)</f>
         <v>4.2420199719614925E-8</v>
       </c>
-      <c r="V3" s="62" t="s">
+      <c r="V3" s="81" t="s">
         <v>41</v>
       </c>
       <c r="X3" s="56">
@@ -6197,11 +6169,14 @@
       <c r="Y3" s="57">
         <v>4.2420199719614925E-8</v>
       </c>
-      <c r="Z3" s="62" t="s">
+      <c r="Z3" s="81" t="s">
         <v>41</v>
       </c>
+      <c r="AA3" s="28">
+        <v>0.37</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -6277,16 +6252,19 @@
         <f t="shared" ref="U4:U50" si="12">((S4*($C$3-$C$9)*$C$4*$C$11)/$C$9)^(1/3)</f>
         <v>5.9531483620197396E-8</v>
       </c>
-      <c r="V4" s="63"/>
+      <c r="V4" s="82"/>
       <c r="X4" s="60">
         <v>5.0784663580564273E-8</v>
       </c>
       <c r="Y4" s="61">
         <v>5.9531483620197396E-8</v>
       </c>
-      <c r="Z4" s="63"/>
+      <c r="Z4" s="82"/>
+      <c r="AA4" s="40">
+        <v>0.44</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -6362,16 +6340,19 @@
         <f t="shared" si="12"/>
         <v>8.3334881356194801E-8</v>
       </c>
-      <c r="V5" s="63"/>
+      <c r="V5" s="82"/>
       <c r="X5" s="60">
         <v>7.0775371384014727E-8</v>
       </c>
       <c r="Y5" s="61">
         <v>8.3334881356194801E-8</v>
       </c>
-      <c r="Z5" s="63"/>
+      <c r="Z5" s="82"/>
+      <c r="AA5" s="40">
+        <v>0.52</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -6447,16 +6428,19 @@
         <f t="shared" si="12"/>
         <v>1.1584807088915935E-7</v>
       </c>
-      <c r="V6" s="63"/>
+      <c r="V6" s="82"/>
       <c r="X6" s="60">
         <v>9.8011193738497813E-8</v>
       </c>
       <c r="Y6" s="61">
         <v>1.1584807088915935E-7</v>
       </c>
-      <c r="Z6" s="63"/>
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="40">
+        <v>0.61</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F7" s="40">
         <v>0.72</v>
       </c>
@@ -6520,24 +6504,27 @@
         <f t="shared" si="12"/>
         <v>1.643246132416318E-7</v>
       </c>
-      <c r="V7" s="63"/>
+      <c r="V7" s="82"/>
       <c r="X7" s="60">
         <v>1.3852698904522814E-7</v>
       </c>
       <c r="Y7" s="61">
         <v>1.643246132416318E-7</v>
       </c>
-      <c r="Z7" s="63"/>
+      <c r="Z7" s="82"/>
+      <c r="AA7" s="40">
+        <v>0.72</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
       <c r="F8" s="40">
         <v>0.85</v>
       </c>
@@ -6601,16 +6588,19 @@
         <f t="shared" si="12"/>
         <v>2.347618303469797E-7</v>
       </c>
-      <c r="V8" s="63"/>
+      <c r="V8" s="82"/>
       <c r="X8" s="60">
         <v>1.9727821119408791E-7</v>
       </c>
       <c r="Y8" s="61">
         <v>2.347618303469797E-7</v>
       </c>
-      <c r="Z8" s="63"/>
+      <c r="Z8" s="82"/>
+      <c r="AA8" s="40">
+        <v>0.85</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>2</v>
       </c>
@@ -6686,16 +6676,19 @@
         <f t="shared" si="12"/>
         <v>3.4224088736910029E-7</v>
       </c>
-      <c r="V9" s="63"/>
+      <c r="V9" s="82"/>
       <c r="X9" s="60">
         <v>2.8676869167901045E-7</v>
       </c>
       <c r="Y9" s="61">
         <v>3.4224088736910029E-7</v>
       </c>
-      <c r="Z9" s="63"/>
+      <c r="Z9" s="82"/>
+      <c r="AA9" s="40">
+        <v>1.01</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -6771,16 +6764,19 @@
         <f t="shared" si="12"/>
         <v>4.9229780900712516E-7</v>
       </c>
-      <c r="V10" s="63"/>
+      <c r="V10" s="82"/>
       <c r="X10" s="60">
         <v>4.1153321700708681E-7</v>
       </c>
       <c r="Y10" s="61">
         <v>4.9229780900712516E-7</v>
       </c>
-      <c r="Z10" s="63"/>
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="40">
+        <v>1.19</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -6857,16 +6853,19 @@
         <f t="shared" si="12"/>
         <v>7.0878057045415601E-7</v>
       </c>
-      <c r="V11" s="63"/>
+      <c r="V11" s="82"/>
       <c r="X11" s="60">
         <v>5.9133240962389227E-7</v>
       </c>
       <c r="Y11" s="61">
         <v>7.0878057045415601E-7</v>
       </c>
-      <c r="Z11" s="63"/>
+      <c r="Z11" s="82"/>
+      <c r="AA11" s="40">
+        <v>1.4</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F12" s="40">
         <v>1.65</v>
       </c>
@@ -6930,24 +6929,27 @@
         <f t="shared" si="12"/>
         <v>1.0281513336458287E-6</v>
       </c>
-      <c r="V12" s="63"/>
+      <c r="V12" s="82"/>
       <c r="X12" s="60">
         <v>8.5637537927746757E-7</v>
       </c>
       <c r="Y12" s="61">
         <v>1.0281513336458287E-6</v>
       </c>
-      <c r="Z12" s="63"/>
+      <c r="Z12" s="82"/>
+      <c r="AA12" s="40">
+        <v>1.65</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
       <c r="F13" s="48">
         <v>1.95</v>
       </c>
@@ -7011,16 +7013,19 @@
         <f t="shared" si="12"/>
         <v>1.5050856358022601E-6</v>
       </c>
-      <c r="V13" s="64"/>
+      <c r="V13" s="83"/>
       <c r="X13" s="58">
         <v>1.2519801324292888E-6</v>
       </c>
       <c r="Y13" s="59">
         <v>1.5050856358022601E-6</v>
       </c>
-      <c r="Z13" s="64"/>
+      <c r="Z13" s="83"/>
+      <c r="AA13" s="48">
+        <v>1.95</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>2</v>
       </c>
@@ -7100,7 +7105,7 @@
         <f t="shared" si="12"/>
         <v>2.1980921686442242E-6</v>
       </c>
-      <c r="V14" s="62" t="s">
+      <c r="V14" s="81" t="s">
         <v>42</v>
       </c>
       <c r="X14" s="56">
@@ -7109,11 +7114,14 @@
       <c r="Y14" s="57">
         <v>2.1980921686442199E-6</v>
       </c>
-      <c r="Z14" s="62" t="s">
+      <c r="Z14" s="81" t="s">
         <v>42</v>
       </c>
+      <c r="AA14" s="28">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
@@ -7189,16 +7197,19 @@
         <f t="shared" si="12"/>
         <v>3.2345524797995237E-6</v>
       </c>
-      <c r="V15" s="63"/>
+      <c r="V15" s="82"/>
       <c r="X15" s="60">
         <v>2.68630965571977E-6</v>
       </c>
       <c r="Y15" s="61">
         <v>3.2345524797995237E-6</v>
       </c>
-      <c r="Z15" s="63"/>
+      <c r="Z15" s="82"/>
+      <c r="AA15" s="40">
+        <v>2.72</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
@@ -7275,16 +7286,19 @@
         <f t="shared" si="12"/>
         <v>4.7067687122065053E-6</v>
       </c>
-      <c r="V16" s="63"/>
+      <c r="V16" s="82"/>
       <c r="X16" s="60">
         <v>3.9077860022104021E-6</v>
       </c>
       <c r="Y16" s="61">
         <v>4.7067687122065053E-6</v>
       </c>
-      <c r="Z16" s="63"/>
+      <c r="Z16" s="82"/>
+      <c r="AA16" s="40">
+        <v>3.2</v>
+      </c>
     </row>
-    <row r="17" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F17" s="40">
         <v>3.78</v>
       </c>
@@ -7348,16 +7362,19 @@
         <f t="shared" si="12"/>
         <v>6.9146758502993435E-6</v>
       </c>
-      <c r="V17" s="63"/>
+      <c r="V17" s="82"/>
       <c r="X17" s="60">
         <v>5.7408451892466158E-6</v>
       </c>
       <c r="Y17" s="61">
         <v>6.9146758502993435E-6</v>
       </c>
-      <c r="Z17" s="63"/>
+      <c r="Z17" s="82"/>
+      <c r="AA17" s="40">
+        <v>3.78</v>
+      </c>
     </row>
-    <row r="18" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F18" s="40">
         <v>4.46</v>
       </c>
@@ -7421,16 +7438,19 @@
         <f t="shared" si="12"/>
         <v>1.012696495395003E-5</v>
       </c>
-      <c r="V18" s="63"/>
+      <c r="V18" s="82"/>
       <c r="X18" s="60">
         <v>8.4102396865991163E-6</v>
       </c>
       <c r="Y18" s="61">
         <v>1.012696495395003E-5</v>
       </c>
-      <c r="Z18" s="63"/>
+      <c r="Z18" s="82"/>
+      <c r="AA18" s="40">
+        <v>4.46</v>
+      </c>
     </row>
-    <row r="19" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F19" s="40">
         <v>5.27</v>
       </c>
@@ -7494,16 +7514,19 @@
         <f t="shared" si="12"/>
         <v>1.4865966732039502E-5</v>
       </c>
-      <c r="V19" s="63"/>
+      <c r="V19" s="82"/>
       <c r="X19" s="60">
         <v>1.235303794633768E-5</v>
       </c>
       <c r="Y19" s="61">
         <v>1.4865966732039502E-5</v>
       </c>
-      <c r="Z19" s="63"/>
+      <c r="Z19" s="82"/>
+      <c r="AA19" s="40">
+        <v>5.27</v>
+      </c>
     </row>
-    <row r="20" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F20" s="40">
         <v>6.21</v>
       </c>
@@ -7567,16 +7590,19 @@
         <f t="shared" si="12"/>
         <v>2.1650592213258089E-5</v>
       </c>
-      <c r="V20" s="63"/>
+      <c r="V20" s="82"/>
       <c r="X20" s="60">
         <v>1.8005947423279784E-5</v>
       </c>
       <c r="Y20" s="61">
         <v>2.1650592213258089E-5</v>
       </c>
-      <c r="Z20" s="63"/>
+      <c r="Z20" s="82"/>
+      <c r="AA20" s="40">
+        <v>6.21</v>
+      </c>
     </row>
-    <row r="21" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F21" s="40">
         <v>7.33</v>
       </c>
@@ -7640,16 +7666,19 @@
         <f t="shared" si="12"/>
         <v>3.1585705119149928E-5</v>
       </c>
-      <c r="V21" s="63"/>
+      <c r="V21" s="82"/>
       <c r="X21" s="60">
         <v>2.62978590045575E-5</v>
       </c>
       <c r="Y21" s="61">
         <v>3.1585705119149928E-5</v>
       </c>
-      <c r="Z21" s="63"/>
+      <c r="Z21" s="82"/>
+      <c r="AA21" s="40">
+        <v>7.33</v>
+      </c>
     </row>
-    <row r="22" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F22" s="40">
         <v>8.65</v>
       </c>
@@ -7713,16 +7742,19 @@
         <f t="shared" si="12"/>
         <v>4.5932628573001273E-5</v>
       </c>
-      <c r="V22" s="63"/>
+      <c r="V22" s="82"/>
       <c r="X22" s="60">
         <v>3.8295168125083617E-5</v>
       </c>
       <c r="Y22" s="61">
         <v>4.5932628573001273E-5</v>
       </c>
-      <c r="Z22" s="63"/>
+      <c r="Z22" s="82"/>
+      <c r="AA22" s="40">
+        <v>8.65</v>
+      </c>
     </row>
-    <row r="23" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F23" s="40">
         <v>10.210000000000001</v>
       </c>
@@ -7786,16 +7818,19 @@
         <f t="shared" si="12"/>
         <v>6.6617763822258673E-5</v>
       </c>
-      <c r="V23" s="63"/>
+      <c r="V23" s="82"/>
       <c r="X23" s="60">
         <v>5.5630342367119438E-5</v>
       </c>
       <c r="Y23" s="61">
         <v>6.6617763822258673E-5</v>
       </c>
-      <c r="Z23" s="63"/>
+      <c r="Z23" s="82"/>
+      <c r="AA23" s="40">
+        <v>10.210000000000001</v>
+      </c>
     </row>
-    <row r="24" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F24" s="40">
         <v>12.05</v>
       </c>
@@ -7859,16 +7894,19 @@
         <f t="shared" si="12"/>
         <v>9.6240773005624341E-5</v>
       </c>
-      <c r="V24" s="63"/>
+      <c r="V24" s="82"/>
       <c r="X24" s="60">
         <v>8.0515572115720573E-5</v>
       </c>
       <c r="Y24" s="61">
         <v>9.6240773005624341E-5</v>
       </c>
-      <c r="Z24" s="63"/>
+      <c r="Z24" s="82"/>
+      <c r="AA24" s="40">
+        <v>12.05</v>
+      </c>
     </row>
-    <row r="25" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F25" s="40">
         <v>14.22</v>
       </c>
@@ -7932,16 +7970,19 @@
         <f t="shared" si="12"/>
         <v>1.3843038121316793E-4</v>
       </c>
-      <c r="V25" s="63"/>
+      <c r="V25" s="82"/>
       <c r="X25" s="60">
         <v>1.1605035140040932E-4</v>
       </c>
       <c r="Y25" s="61">
         <v>1.3843038121316793E-4</v>
       </c>
-      <c r="Z25" s="63"/>
+      <c r="Z25" s="82"/>
+      <c r="AA25" s="40">
+        <v>14.22</v>
+      </c>
     </row>
-    <row r="26" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F26" s="40">
         <v>16.78</v>
       </c>
@@ -8005,16 +8046,19 @@
         <f t="shared" si="12"/>
         <v>1.981905350973394E-4</v>
       </c>
-      <c r="V26" s="63"/>
+      <c r="V26" s="82"/>
       <c r="X26" s="60">
         <v>1.6652632125677697E-4</v>
       </c>
       <c r="Y26" s="61">
         <v>1.981905350973394E-4</v>
       </c>
-      <c r="Z26" s="63"/>
+      <c r="Z26" s="82"/>
+      <c r="AA26" s="40">
+        <v>16.78</v>
+      </c>
     </row>
-    <row r="27" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F27" s="48">
         <v>19.809999999999999</v>
       </c>
@@ -8078,16 +8122,19 @@
         <f t="shared" si="12"/>
         <v>2.8262028985907259E-4</v>
       </c>
-      <c r="V27" s="64"/>
+      <c r="V27" s="83"/>
       <c r="X27" s="58">
         <v>2.3805512943131894E-4</v>
       </c>
       <c r="Y27" s="59">
         <v>2.8262028985907259E-4</v>
       </c>
-      <c r="Z27" s="64"/>
+      <c r="Z27" s="83"/>
+      <c r="AA27" s="48">
+        <v>19.809999999999999</v>
+      </c>
     </row>
-    <row r="28" spans="5:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E28">
         <f>F28/1000</f>
         <v>2.3370000000000002E-2</v>
@@ -8151,24 +8198,27 @@
         <f t="shared" si="11"/>
         <v>3.3802201988097691E-4</v>
       </c>
-      <c r="U28" s="72">
+      <c r="U28" s="62">
         <f t="shared" si="12"/>
         <v>4.0023945736018736E-4</v>
       </c>
-      <c r="V28" s="75" t="s">
+      <c r="V28" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="X28" s="98">
+      <c r="X28" s="73">
         <v>3.3802201988097702E-4</v>
       </c>
-      <c r="Y28" s="99">
+      <c r="Y28" s="74">
         <v>4.0023945736018698E-4</v>
       </c>
-      <c r="Z28" s="65" t="s">
+      <c r="Z28" s="86" t="s">
         <v>43</v>
       </c>
+      <c r="AA28" s="28">
+        <v>23.37</v>
+      </c>
     </row>
-    <row r="29" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F29" s="40">
         <v>27.58</v>
       </c>
@@ -8228,20 +8278,23 @@
         <f t="shared" si="11"/>
         <v>4.7768872833639395E-4</v>
       </c>
-      <c r="U29" s="73">
+      <c r="U29" s="63">
         <f t="shared" si="12"/>
         <v>5.640136783750916E-4</v>
       </c>
-      <c r="V29" s="76"/>
-      <c r="X29" s="100">
+      <c r="V29" s="85"/>
+      <c r="X29" s="75">
         <v>4.7768872833639395E-4</v>
       </c>
-      <c r="Y29" s="101">
+      <c r="Y29" s="76">
         <v>5.640136783750916E-4</v>
       </c>
-      <c r="Z29" s="66"/>
+      <c r="Z29" s="87"/>
+      <c r="AA29" s="40">
+        <v>27.58</v>
+      </c>
     </row>
-    <row r="30" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F30" s="40">
         <v>32.549999999999997</v>
       </c>
@@ -8301,20 +8354,23 @@
         <f t="shared" si="11"/>
         <v>6.7115100953837078E-4</v>
       </c>
-      <c r="U30" s="73">
+      <c r="U30" s="63">
         <f t="shared" si="12"/>
         <v>7.9006357794236478E-4</v>
       </c>
-      <c r="V30" s="76"/>
-      <c r="X30" s="100">
+      <c r="V30" s="85"/>
+      <c r="X30" s="75">
         <v>6.7115100953837078E-4</v>
       </c>
-      <c r="Y30" s="101">
+      <c r="Y30" s="76">
         <v>7.9006357794236478E-4</v>
       </c>
-      <c r="Z30" s="66"/>
+      <c r="Z30" s="87"/>
+      <c r="AA30" s="40">
+        <v>32.549999999999997</v>
+      </c>
     </row>
-    <row r="31" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F31" s="40">
         <v>38.409999999999997</v>
       </c>
@@ -8374,20 +8430,23 @@
         <f t="shared" si="11"/>
         <v>9.3681445776628018E-4</v>
       </c>
-      <c r="U31" s="73">
+      <c r="U31" s="63">
         <f t="shared" si="12"/>
         <v>1.0993252704586346E-3</v>
       </c>
-      <c r="V31" s="76"/>
-      <c r="X31" s="100">
+      <c r="V31" s="85"/>
+      <c r="X31" s="75">
         <v>9.3681445776628018E-4</v>
       </c>
-      <c r="Y31" s="101">
+      <c r="Y31" s="76">
         <v>1.0993252704586346E-3</v>
       </c>
-      <c r="Z31" s="66"/>
+      <c r="Z31" s="87"/>
+      <c r="AA31" s="40">
+        <v>38.409999999999997</v>
+      </c>
     </row>
-    <row r="32" spans="5:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:27" x14ac:dyDescent="0.3">
       <c r="F32" s="40">
         <v>45.32</v>
       </c>
@@ -8447,20 +8506,23 @@
         <f t="shared" si="11"/>
         <v>1.2988139297590265E-3</v>
       </c>
-      <c r="U32" s="73">
+      <c r="U32" s="63">
         <f t="shared" si="12"/>
         <v>1.5191077279832483E-3</v>
       </c>
-      <c r="V32" s="76"/>
-      <c r="X32" s="100">
+      <c r="V32" s="85"/>
+      <c r="X32" s="75">
         <v>1.2988139297590265E-3</v>
       </c>
-      <c r="Y32" s="101">
+      <c r="Y32" s="76">
         <v>1.5191077279832483E-3</v>
       </c>
-      <c r="Z32" s="66"/>
+      <c r="Z32" s="87"/>
+      <c r="AA32" s="40">
+        <v>45.32</v>
+      </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F33" s="40">
         <v>53.48</v>
       </c>
@@ -8520,20 +8582,23 @@
         <f t="shared" si="11"/>
         <v>1.7888665047406367E-3</v>
       </c>
-      <c r="U33" s="73">
+      <c r="U33" s="63">
         <f t="shared" si="12"/>
         <v>2.0851114422061512E-3</v>
       </c>
-      <c r="V33" s="76"/>
-      <c r="X33" s="100">
+      <c r="V33" s="85"/>
+      <c r="X33" s="75">
         <v>1.7888665047406367E-3</v>
       </c>
-      <c r="Y33" s="101">
+      <c r="Y33" s="76">
         <v>2.0851114422061512E-3</v>
       </c>
-      <c r="Z33" s="66"/>
+      <c r="Z33" s="87"/>
+      <c r="AA33" s="40">
+        <v>53.48</v>
+      </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F34" s="40">
         <v>63.11</v>
       </c>
@@ -8593,20 +8658,23 @@
         <f t="shared" si="11"/>
         <v>2.446401268148512E-3</v>
       </c>
-      <c r="U34" s="73">
+      <c r="U34" s="63">
         <f t="shared" si="12"/>
         <v>2.8414167636944148E-3</v>
       </c>
-      <c r="V34" s="76"/>
-      <c r="X34" s="100">
+      <c r="V34" s="85"/>
+      <c r="X34" s="75">
         <v>2.446401268148512E-3</v>
       </c>
-      <c r="Y34" s="101">
+      <c r="Y34" s="76">
         <v>2.8414167636944148E-3</v>
       </c>
-      <c r="Z34" s="66"/>
+      <c r="Z34" s="87"/>
+      <c r="AA34" s="40">
+        <v>63.11</v>
+      </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F35" s="40">
         <v>74.48</v>
       </c>
@@ -8666,20 +8734,23 @@
         <f t="shared" si="11"/>
         <v>3.3215531046029726E-3</v>
       </c>
-      <c r="U35" s="73">
+      <c r="U35" s="63">
         <f t="shared" si="12"/>
         <v>3.8437427395106539E-3</v>
       </c>
-      <c r="V35" s="76"/>
-      <c r="X35" s="100">
+      <c r="V35" s="85"/>
+      <c r="X35" s="75">
         <v>3.3215531046029726E-3</v>
       </c>
-      <c r="Y35" s="101">
+      <c r="Y35" s="76">
         <v>3.8437427395106539E-3</v>
       </c>
-      <c r="Z35" s="66"/>
+      <c r="Z35" s="87"/>
+      <c r="AA35" s="40">
+        <v>74.48</v>
+      </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F36" s="40">
         <v>87.89</v>
       </c>
@@ -8739,20 +8810,23 @@
         <f t="shared" si="11"/>
         <v>4.4748544960825096E-3</v>
       </c>
-      <c r="U36" s="73">
+      <c r="U36" s="63">
         <f t="shared" si="12"/>
         <v>5.1588611284876969E-3</v>
       </c>
-      <c r="V36" s="76"/>
-      <c r="X36" s="100">
+      <c r="V36" s="85"/>
+      <c r="X36" s="75">
         <v>4.4748544960825096E-3</v>
       </c>
-      <c r="Y36" s="101">
+      <c r="Y36" s="76">
         <v>5.1588611284876969E-3</v>
       </c>
-      <c r="Z36" s="66"/>
+      <c r="Z36" s="87"/>
+      <c r="AA36" s="40">
+        <v>87.89</v>
+      </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F37" s="40">
         <v>103.72</v>
       </c>
@@ -8812,20 +8886,23 @@
         <f t="shared" si="11"/>
         <v>5.9823072602970774E-3</v>
       </c>
-      <c r="U37" s="73">
+      <c r="U37" s="63">
         <f t="shared" si="12"/>
         <v>6.8701142126075532E-3</v>
       </c>
-      <c r="V37" s="76"/>
-      <c r="X37" s="100">
+      <c r="V37" s="85"/>
+      <c r="X37" s="75">
         <v>5.9823072602970774E-3</v>
       </c>
-      <c r="Y37" s="101">
+      <c r="Y37" s="76">
         <v>6.8701142126075532E-3</v>
       </c>
-      <c r="Z37" s="66"/>
+      <c r="Z37" s="87"/>
+      <c r="AA37" s="40">
+        <v>103.72</v>
+      </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F38" s="40">
         <v>122.39</v>
       </c>
@@ -8885,20 +8962,23 @@
         <f t="shared" si="11"/>
         <v>7.9326709248603178E-3</v>
       </c>
-      <c r="U38" s="73">
+      <c r="U38" s="63">
         <f t="shared" si="12"/>
         <v>9.0739978516363538E-3</v>
       </c>
-      <c r="V38" s="76"/>
-      <c r="X38" s="100">
+      <c r="V38" s="85"/>
+      <c r="X38" s="75">
         <v>7.9326709248603178E-3</v>
       </c>
-      <c r="Y38" s="101">
+      <c r="Y38" s="76">
         <v>9.0739978516363538E-3</v>
       </c>
-      <c r="Z38" s="66"/>
+      <c r="Z38" s="87"/>
+      <c r="AA38" s="40">
+        <v>122.39</v>
+      </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F39" s="40">
         <v>144.43</v>
       </c>
@@ -8958,72 +9038,75 @@
         <f t="shared" si="11"/>
         <v>1.0434519051762263E-2</v>
       </c>
-      <c r="U39" s="73">
+      <c r="U39" s="63">
         <f t="shared" si="12"/>
         <v>1.188778207941428E-2</v>
       </c>
-      <c r="V39" s="76"/>
-      <c r="X39" s="100">
+      <c r="V39" s="85"/>
+      <c r="X39" s="75">
         <v>1.0434519051762263E-2</v>
       </c>
-      <c r="Y39" s="101">
+      <c r="Y39" s="76">
         <v>1.188778207941428E-2</v>
       </c>
-      <c r="Z39" s="66"/>
+      <c r="Z39" s="87"/>
+      <c r="AA39" s="40">
+        <v>144.43</v>
+      </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F40" s="40">
         <v>170.44</v>
       </c>
-      <c r="G40" s="78">
+      <c r="G40" s="41">
         <f t="shared" si="1"/>
         <v>1.7044E-4</v>
       </c>
-      <c r="H40" s="79">
+      <c r="H40" s="42">
         <f t="shared" si="15"/>
         <v>39.434579036756475</v>
       </c>
-      <c r="I40" s="80">
+      <c r="I40" s="43">
         <f t="shared" si="0"/>
         <v>50.217472429632487</v>
       </c>
-      <c r="J40" s="81">
+      <c r="J40" s="44">
         <f t="shared" si="2"/>
         <v>-0.9577095308956306</v>
       </c>
-      <c r="K40" s="79">
+      <c r="K40" s="42">
         <f t="shared" si="3"/>
         <v>-5.0704833844959817E-3</v>
       </c>
-      <c r="L40" s="82">
+      <c r="L40" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M40" s="83">
+      <c r="M40" s="45">
         <f t="shared" si="14"/>
         <v>0.99810753012424036</v>
       </c>
-      <c r="N40" s="84">
+      <c r="N40" s="46">
         <f t="shared" si="5"/>
         <v>-0.79299725925593822</v>
       </c>
-      <c r="O40" s="80">
+      <c r="O40" s="43">
         <f t="shared" si="6"/>
         <v>-5.0720552514615883E-3</v>
       </c>
-      <c r="P40" s="85">
+      <c r="P40" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q40" s="86">
+      <c r="Q40" s="47">
         <f t="shared" si="8"/>
         <v>0.99770789395747417</v>
       </c>
-      <c r="R40" s="79">
+      <c r="R40" s="42">
         <f t="shared" si="9"/>
         <v>0.10874200036583882</v>
       </c>
-      <c r="S40" s="80">
+      <c r="S40" s="43">
         <f t="shared" si="10"/>
         <v>0.1588305697934522</v>
       </c>
@@ -9031,20 +9114,23 @@
         <f t="shared" si="11"/>
         <v>1.3611766542267135E-2</v>
       </c>
-      <c r="U40" s="73">
+      <c r="U40" s="63">
         <f t="shared" si="12"/>
         <v>1.5444010344976085E-2</v>
       </c>
-      <c r="V40" s="76"/>
-      <c r="X40" s="100">
+      <c r="V40" s="85"/>
+      <c r="X40" s="75">
         <v>1.3611766542267135E-2</v>
       </c>
-      <c r="Y40" s="101">
+      <c r="Y40" s="76">
         <v>1.5444010344976085E-2</v>
       </c>
-      <c r="Z40" s="67"/>
+      <c r="Z40" s="88"/>
+      <c r="AA40" s="40">
+        <v>170.44</v>
+      </c>
     </row>
-    <row r="41" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
         <v>40</v>
       </c>
@@ -9107,76 +9193,79 @@
         <f t="shared" si="11"/>
         <v>1.7606088561399769E-2</v>
       </c>
-      <c r="U41" s="72">
+      <c r="U41" s="62">
         <f t="shared" si="12"/>
         <v>1.9892755414532847E-2</v>
       </c>
-      <c r="V41" s="75" t="s">
+      <c r="V41" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="X41" s="91">
+      <c r="X41" s="67">
         <v>1.7606088561399801E-2</v>
       </c>
-      <c r="Y41" s="92">
+      <c r="Y41" s="68">
         <v>1.9892755414532799E-2</v>
       </c>
-      <c r="Z41" s="65" t="s">
+      <c r="Z41" s="86" t="s">
         <v>44</v>
       </c>
+      <c r="AA41" s="28">
+        <v>201.13</v>
+      </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F42" s="40">
         <v>237.35</v>
       </c>
-      <c r="G42" s="78">
+      <c r="G42" s="41">
         <f t="shared" si="1"/>
         <v>2.3735E-4</v>
       </c>
-      <c r="H42" s="79">
+      <c r="H42" s="42">
         <f t="shared" si="15"/>
         <v>106.49527532568401</v>
       </c>
-      <c r="I42" s="80">
+      <c r="I42" s="43">
         <f t="shared" si="0"/>
         <v>135.61507902921761</v>
       </c>
-      <c r="J42" s="81">
+      <c r="J42" s="44">
         <f t="shared" si="2"/>
         <v>-0.29739274225782858</v>
       </c>
-      <c r="K42" s="79">
+      <c r="K42" s="42">
         <f t="shared" si="3"/>
         <v>-5.0769935584841826E-3</v>
       </c>
-      <c r="L42" s="82">
+      <c r="L42" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M42" s="83">
+      <c r="M42" s="45">
         <f t="shared" si="14"/>
         <v>0.99577044655892555</v>
       </c>
-      <c r="N42" s="84">
+      <c r="N42" s="46">
         <f t="shared" si="5"/>
         <v>-0.14342168239242972</v>
       </c>
-      <c r="O42" s="80">
+      <c r="O42" s="43">
         <f t="shared" si="6"/>
         <v>-5.0786042322366132E-3</v>
       </c>
-      <c r="P42" s="85">
+      <c r="P42" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q42" s="86">
+      <c r="Q42" s="47">
         <f t="shared" si="8"/>
         <v>0.99483035924374286</v>
       </c>
-      <c r="R42" s="79">
+      <c r="R42" s="42">
         <f t="shared" si="9"/>
         <v>0.49623740479131878</v>
       </c>
-      <c r="S42" s="80">
+      <c r="S42" s="43">
         <f t="shared" si="10"/>
         <v>0.70672221575801508</v>
       </c>
@@ -9184,72 +9273,75 @@
         <f t="shared" si="11"/>
         <v>2.2577640394208058E-2</v>
       </c>
-      <c r="U42" s="73">
+      <c r="U42" s="63">
         <f t="shared" si="12"/>
         <v>2.5401827769121761E-2</v>
       </c>
-      <c r="V42" s="76"/>
-      <c r="X42" s="93">
+      <c r="V42" s="85"/>
+      <c r="X42" s="69">
         <v>2.2577640394208058E-2</v>
       </c>
-      <c r="Y42" s="94">
+      <c r="Y42" s="70">
         <v>2.5401827769121761E-2</v>
       </c>
-      <c r="Z42" s="66"/>
+      <c r="Z42" s="87"/>
+      <c r="AA42" s="40">
+        <v>237.35</v>
+      </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F43" s="40">
         <v>280.08999999999997</v>
       </c>
-      <c r="G43" s="78">
+      <c r="G43" s="41">
         <f t="shared" si="1"/>
         <v>2.8008999999999998E-4</v>
       </c>
-      <c r="H43" s="79">
+      <c r="H43" s="42">
         <f t="shared" si="15"/>
         <v>175.00700930888829</v>
       </c>
-      <c r="I43" s="80">
+      <c r="I43" s="43">
         <f t="shared" si="0"/>
         <v>222.86049146790603</v>
       </c>
-      <c r="J43" s="81">
+      <c r="J43" s="44">
         <f t="shared" si="2"/>
         <v>1.6153330292586823E-2</v>
       </c>
-      <c r="K43" s="79">
+      <c r="K43" s="42">
         <f t="shared" si="3"/>
         <v>-5.0803203206637613E-3</v>
       </c>
-      <c r="L43" s="82">
+      <c r="L43" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M43" s="83">
+      <c r="M43" s="45">
         <f t="shared" si="14"/>
         <v>0.99360340517183265</v>
       </c>
-      <c r="N43" s="84">
+      <c r="N43" s="46">
         <f t="shared" si="5"/>
         <v>0.16469875961089339</v>
       </c>
-      <c r="O43" s="80">
+      <c r="O43" s="43">
         <f t="shared" si="6"/>
         <v>-5.0819666901397035E-3</v>
       </c>
-      <c r="P43" s="85">
+      <c r="P43" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q43" s="86">
+      <c r="Q43" s="47">
         <f t="shared" si="8"/>
         <v>0.99216619360742264</v>
       </c>
-      <c r="R43" s="79">
+      <c r="R43" s="42">
         <f t="shared" si="9"/>
         <v>1.0192625819801655</v>
       </c>
-      <c r="S43" s="80">
+      <c r="S43" s="43">
         <f t="shared" si="10"/>
         <v>1.4328516166261867</v>
       </c>
@@ -9257,72 +9349,75 @@
         <f t="shared" si="11"/>
         <v>2.8699703694252371E-2</v>
       </c>
-      <c r="U43" s="73">
+      <c r="U43" s="63">
         <f t="shared" si="12"/>
         <v>3.2150109658340281E-2</v>
       </c>
-      <c r="V43" s="76"/>
-      <c r="X43" s="93">
+      <c r="V43" s="85"/>
+      <c r="X43" s="69">
         <v>2.8699703694252371E-2</v>
       </c>
-      <c r="Y43" s="94">
+      <c r="Y43" s="70">
         <v>3.2150109658340281E-2</v>
       </c>
-      <c r="Z43" s="66"/>
+      <c r="Z43" s="87"/>
+      <c r="AA43" s="40">
+        <v>280.08999999999997</v>
+      </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F44" s="40">
         <v>330.52</v>
       </c>
-      <c r="G44" s="78">
+      <c r="G44" s="41">
         <f t="shared" si="1"/>
         <v>3.3051999999999995E-4</v>
       </c>
-      <c r="H44" s="79">
+      <c r="H44" s="42">
         <f t="shared" si="15"/>
         <v>287.57813623849836</v>
       </c>
-      <c r="I44" s="80">
+      <c r="I44" s="43">
         <f t="shared" si="0"/>
         <v>366.21278787992628</v>
       </c>
-      <c r="J44" s="81">
+      <c r="J44" s="44">
         <f t="shared" si="2"/>
         <v>0.31850472858852219</v>
       </c>
-      <c r="K44" s="79">
+      <c r="K44" s="42">
         <f t="shared" si="3"/>
         <v>-5.0837287466916356E-3</v>
       </c>
-      <c r="L44" s="82">
+      <c r="L44" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M44" s="83">
+      <c r="M44" s="45">
         <f t="shared" si="14"/>
         <v>0.99029400169885529</v>
       </c>
-      <c r="N44" s="84">
+      <c r="N44" s="46">
         <f t="shared" si="5"/>
         <v>0.46160732932345383</v>
       </c>
-      <c r="O44" s="80">
+      <c r="O44" s="43">
         <f t="shared" si="6"/>
         <v>-5.0854290964561623E-3</v>
       </c>
-      <c r="P44" s="85">
+      <c r="P44" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q44" s="86">
+      <c r="Q44" s="47">
         <f t="shared" si="8"/>
         <v>0.98810502191697325</v>
       </c>
-      <c r="R44" s="79">
+      <c r="R44" s="42">
         <f t="shared" si="9"/>
         <v>2.0379106942263467</v>
       </c>
-      <c r="S44" s="80">
+      <c r="S44" s="43">
         <f t="shared" si="10"/>
         <v>2.8269947813060363</v>
       </c>
@@ -9330,72 +9425,75 @@
         <f t="shared" si="11"/>
         <v>3.6155727290167847E-2</v>
       </c>
-      <c r="U44" s="73">
+      <c r="U44" s="63">
         <f t="shared" si="12"/>
         <v>4.0323391724231661E-2</v>
       </c>
-      <c r="V44" s="76"/>
-      <c r="X44" s="93">
+      <c r="V44" s="85"/>
+      <c r="X44" s="69">
         <v>3.6155727290167847E-2</v>
       </c>
-      <c r="Y44" s="94">
+      <c r="Y44" s="70">
         <v>4.0323391724231661E-2</v>
       </c>
-      <c r="Z44" s="66"/>
+      <c r="Z44" s="87"/>
+      <c r="AA44" s="40">
+        <v>330.52</v>
+      </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F45" s="40">
         <v>390.04</v>
       </c>
-      <c r="G45" s="78">
+      <c r="G45" s="41">
         <f t="shared" si="1"/>
         <v>3.9004000000000003E-4</v>
       </c>
-      <c r="H45" s="79">
+      <c r="H45" s="42">
         <f t="shared" si="15"/>
         <v>472.5960373517471</v>
       </c>
-      <c r="I45" s="80">
+      <c r="I45" s="43">
         <f t="shared" si="0"/>
         <v>601.82152455448011</v>
       </c>
-      <c r="J45" s="81">
+      <c r="J45" s="44">
         <f t="shared" si="2"/>
         <v>0.60971355350193235</v>
       </c>
-      <c r="K45" s="79">
+      <c r="K45" s="42">
         <f t="shared" si="3"/>
         <v>-5.0872615180391628E-3</v>
       </c>
-      <c r="L45" s="82">
+      <c r="L45" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M45" s="83">
+      <c r="M45" s="45">
         <f t="shared" si="14"/>
         <v>0.98525979359254012</v>
       </c>
-      <c r="N45" s="84">
+      <c r="N45" s="46">
         <f t="shared" si="5"/>
         <v>0.74736881523089904</v>
       </c>
-      <c r="O45" s="80">
+      <c r="O45" s="43">
         <f t="shared" si="6"/>
         <v>-5.0890427518031694E-3</v>
       </c>
-      <c r="P45" s="85">
+      <c r="P45" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q45" s="86">
+      <c r="Q45" s="47">
         <f t="shared" si="8"/>
         <v>0.98194436521791539</v>
       </c>
-      <c r="R45" s="79">
+      <c r="R45" s="42">
         <f t="shared" si="9"/>
         <v>3.964396211851823</v>
       </c>
-      <c r="S45" s="80">
+      <c r="S45" s="43">
         <f t="shared" si="10"/>
         <v>5.4245866997395291</v>
       </c>
@@ -9403,312 +9501,327 @@
         <f t="shared" si="11"/>
         <v>4.5134406571575331E-2</v>
       </c>
-      <c r="U45" s="73">
+      <c r="U45" s="63">
         <f t="shared" si="12"/>
         <v>5.010767718220193E-2</v>
       </c>
-      <c r="V45" s="76"/>
-      <c r="X45" s="93">
+      <c r="V45" s="85"/>
+      <c r="X45" s="69">
         <v>4.5134406571575331E-2</v>
       </c>
-      <c r="Y45" s="94">
+      <c r="Y45" s="70">
         <v>5.010767718220193E-2</v>
       </c>
-      <c r="Z45" s="66"/>
+      <c r="Z45" s="87"/>
+      <c r="AA45" s="40">
+        <v>390.04</v>
+      </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F46" s="40">
         <v>460.27</v>
       </c>
-      <c r="G46" s="78">
+      <c r="G46" s="41">
         <f>F46*0.000001</f>
         <v>4.6026999999999998E-4</v>
       </c>
-      <c r="H46" s="79">
+      <c r="H46" s="42">
         <f t="shared" si="15"/>
         <v>776.60581689290984</v>
       </c>
-      <c r="I46" s="80">
+      <c r="I46" s="43">
         <f t="shared" si="0"/>
         <v>988.95898348911669</v>
       </c>
-      <c r="J46" s="81">
+      <c r="J46" s="44">
         <f t="shared" si="2"/>
         <v>0.88970143866050433</v>
       </c>
-      <c r="K46" s="79">
+      <c r="K46" s="42">
         <f t="shared" si="3"/>
         <v>-5.0909786977164605E-3</v>
       </c>
-      <c r="L46" s="82">
+      <c r="L46" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M46" s="83">
+      <c r="M46" s="45">
         <f>(0.65-(($C$5/2.83)*TANH(LOG10(H46)-4.6)))^L46</f>
         <v>0.97765254159064829</v>
       </c>
-      <c r="N46" s="84">
+      <c r="N46" s="46">
         <f t="shared" si="5"/>
         <v>1.0219204636120567</v>
       </c>
-      <c r="O46" s="80">
+      <c r="O46" s="43">
         <f t="shared" si="6"/>
         <v>-5.0928793553075757E-3</v>
       </c>
-      <c r="P46" s="85">
+      <c r="P46" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q46" s="86">
+      <c r="Q46" s="47">
         <f>(0.65-(($C$5/2.83)*TANH(LOG10(I46)-4.6)))^P46</f>
         <v>0.97267393134013647</v>
       </c>
-      <c r="R46" s="79">
+      <c r="R46" s="42">
         <f t="shared" si="9"/>
         <v>7.4954030930103857</v>
       </c>
-      <c r="S46" s="80">
+      <c r="S46" s="43">
         <f t="shared" si="10"/>
         <v>10.111017469510898</v>
       </c>
-      <c r="T46" s="88">
+      <c r="T46" s="65">
         <f t="shared" si="11"/>
         <v>5.5810217765736178E-2</v>
       </c>
-      <c r="U46" s="73">
+      <c r="U46" s="63">
         <f t="shared" si="12"/>
         <v>6.1666174302810024E-2</v>
       </c>
-      <c r="V46" s="76"/>
-      <c r="X46" s="93">
+      <c r="V46" s="85"/>
+      <c r="X46" s="69">
         <v>5.5810217765736178E-2</v>
       </c>
-      <c r="Y46" s="94">
+      <c r="Y46" s="70">
         <v>6.1666174302810024E-2</v>
       </c>
-      <c r="Z46" s="66"/>
+      <c r="Z46" s="87"/>
+      <c r="AA46" s="40">
+        <v>460.27</v>
+      </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F47" s="40">
         <v>500</v>
       </c>
-      <c r="G47" s="78">
+      <c r="G47" s="41">
         <f t="shared" ref="G47:G50" si="16">F47*0.000001</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H47" s="79">
+      <c r="H47" s="42">
         <f t="shared" si="15"/>
         <v>995.5719352354572</v>
       </c>
-      <c r="I47" s="80">
+      <c r="I47" s="43">
         <f t="shared" si="0"/>
         <v>1267.7986536334677</v>
       </c>
-      <c r="J47" s="81">
+      <c r="J47" s="44">
         <f t="shared" si="2"/>
         <v>1.0255285151092788</v>
       </c>
-      <c r="K47" s="79">
+      <c r="K47" s="42">
         <f t="shared" si="3"/>
         <v>-5.0929327784093818E-3</v>
       </c>
-      <c r="L47" s="82">
+      <c r="L47" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M47" s="83">
+      <c r="M47" s="45">
         <f t="shared" ref="M47:M50" si="17">(0.65-(($C$5/2.83)*TANH(LOG10(H47)-4.6)))^L47</f>
         <v>0.97252246538758746</v>
       </c>
-      <c r="N47" s="84">
+      <c r="N47" s="46">
         <f t="shared" si="5"/>
         <v>1.1550373669278229</v>
       </c>
-      <c r="O47" s="80">
+      <c r="O47" s="43">
         <f t="shared" si="6"/>
         <v>-5.0949120794334694E-3</v>
       </c>
-      <c r="P47" s="85">
+      <c r="P47" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q47" s="86">
+      <c r="Q47" s="47">
         <f t="shared" ref="Q47:Q50" si="18">(0.65-(($C$5/2.83)*TANH(LOG10(I47)-4.6)))^P47</f>
         <v>0.966448610280638</v>
       </c>
-      <c r="R47" s="79">
+      <c r="R47" s="42">
         <f t="shared" si="9"/>
         <v>10.193779253533988</v>
       </c>
-      <c r="S47" s="80">
+      <c r="S47" s="43">
         <f t="shared" si="10"/>
         <v>13.649640736870976</v>
       </c>
-      <c r="T47" s="88">
+      <c r="T47" s="65">
         <f t="shared" si="11"/>
         <v>6.1833969507105138E-2</v>
       </c>
-      <c r="U47" s="73">
+      <c r="U47" s="63">
         <f t="shared" si="12"/>
         <v>6.8153651021235329E-2</v>
       </c>
-      <c r="V47" s="76"/>
-      <c r="X47" s="93">
+      <c r="V47" s="85"/>
+      <c r="X47" s="69">
         <v>6.1833969507105138E-2</v>
       </c>
-      <c r="Y47" s="95">
+      <c r="Y47" s="70">
         <v>6.8153651021235329E-2</v>
       </c>
-      <c r="Z47" s="66"/>
+      <c r="Z47" s="87"/>
+      <c r="AA47" s="40">
+        <v>500</v>
+      </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F48" s="40">
         <v>700</v>
       </c>
-      <c r="G48" s="78">
+      <c r="G48" s="41">
         <f t="shared" si="16"/>
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="H48" s="79">
+      <c r="H48" s="42">
         <f t="shared" si="15"/>
         <v>2731.8493902860937</v>
       </c>
-      <c r="I48" s="80">
+      <c r="I48" s="43">
         <f t="shared" si="0"/>
         <v>3478.8395055702345</v>
       </c>
-      <c r="J48" s="81">
+      <c r="J48" s="44">
         <f t="shared" si="2"/>
         <v>1.5489611268405998</v>
       </c>
-      <c r="K48" s="79">
+      <c r="K48" s="42">
         <f t="shared" si="3"/>
         <v>-5.1018830562647183E-3</v>
       </c>
-      <c r="L48" s="82">
+      <c r="L48" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M48" s="83">
+      <c r="M48" s="45">
         <f t="shared" si="17"/>
         <v>0.93762167345962177</v>
       </c>
-      <c r="N48" s="84">
+      <c r="N48" s="46">
         <f t="shared" si="5"/>
         <v>1.6675563367886639</v>
       </c>
-      <c r="O48" s="80">
+      <c r="O48" s="43">
         <f t="shared" si="6"/>
         <v>-5.1043575596395069E-3</v>
       </c>
-      <c r="P48" s="85">
+      <c r="P48" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q48" s="86">
+      <c r="Q48" s="47">
         <f t="shared" si="18"/>
         <v>0.92465127522114177</v>
       </c>
-      <c r="R48" s="79">
+      <c r="R48" s="42">
         <f t="shared" si="9"/>
         <v>32.800984686965492</v>
       </c>
-      <c r="S48" s="80">
+      <c r="S48" s="43">
         <f t="shared" si="10"/>
         <v>42.504014609887193</v>
       </c>
-      <c r="T48" s="88">
+      <c r="T48" s="65">
         <f t="shared" si="11"/>
         <v>9.128743681273252E-2</v>
       </c>
-      <c r="U48" s="73">
+      <c r="U48" s="63">
         <f t="shared" si="12"/>
         <v>9.9523437955351138E-2</v>
       </c>
-      <c r="V48" s="76"/>
-      <c r="X48" s="93">
+      <c r="V48" s="85"/>
+      <c r="X48" s="69">
         <v>9.128743681273252E-2</v>
       </c>
-      <c r="Y48" s="95">
+      <c r="Y48" s="70">
         <v>9.9523437955351138E-2</v>
       </c>
-      <c r="Z48" s="66"/>
+      <c r="Z48" s="87"/>
+      <c r="AA48" s="40">
+        <v>700</v>
+      </c>
     </row>
-    <row r="49" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:27" x14ac:dyDescent="0.3">
       <c r="F49" s="40">
         <v>1000</v>
       </c>
-      <c r="G49" s="78">
+      <c r="G49" s="41">
         <f t="shared" si="16"/>
         <v>1E-3</v>
       </c>
-      <c r="H49" s="79">
+      <c r="H49" s="42">
         <f t="shared" si="15"/>
         <v>7964.5754818836576</v>
       </c>
-      <c r="I49" s="80">
+      <c r="I49" s="43">
         <f t="shared" si="0"/>
         <v>10142.389229067741</v>
       </c>
-      <c r="J49" s="81">
+      <c r="J49" s="44">
         <f t="shared" si="2"/>
         <v>2.0544753860698988</v>
       </c>
-      <c r="K49" s="79">
+      <c r="K49" s="42">
         <f t="shared" si="3"/>
         <v>-5.1142042608855187E-3</v>
       </c>
-      <c r="L49" s="82">
+      <c r="L49" s="16">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M49" s="83">
+      <c r="M49" s="45">
         <f t="shared" si="17"/>
         <v>0.86116360309606788</v>
       </c>
-      <c r="N49" s="84">
+      <c r="N49" s="46">
         <f t="shared" si="5"/>
         <v>2.1617772259948014</v>
       </c>
-      <c r="O49" s="80">
+      <c r="O49" s="43">
         <f t="shared" si="6"/>
         <v>-5.1175299523507703E-3</v>
       </c>
-      <c r="P49" s="85">
+      <c r="P49" s="17">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q49" s="86">
+      <c r="Q49" s="47">
         <f t="shared" si="18"/>
         <v>0.83633894897489802</v>
       </c>
-      <c r="R49" s="79">
+      <c r="R49" s="42">
         <f t="shared" si="9"/>
         <v>96.482122295880757</v>
       </c>
-      <c r="S49" s="80">
+      <c r="S49" s="43">
         <f t="shared" si="10"/>
         <v>119.96153623901775</v>
       </c>
-      <c r="T49" s="88">
+      <c r="T49" s="65">
         <f t="shared" si="11"/>
         <v>0.13079696553398346</v>
       </c>
-      <c r="U49" s="73">
+      <c r="U49" s="63">
         <f t="shared" si="12"/>
         <v>0.14064664992895701</v>
       </c>
-      <c r="V49" s="76"/>
-      <c r="X49" s="93">
+      <c r="V49" s="85"/>
+      <c r="X49" s="69">
         <v>0.13079696553398346</v>
       </c>
-      <c r="Y49" s="95">
+      <c r="Y49" s="70">
         <v>0.14064664992895701</v>
       </c>
-      <c r="Z49" s="66"/>
+      <c r="Z49" s="87"/>
+      <c r="AA49" s="40">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="50" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:27" x14ac:dyDescent="0.3">
       <c r="F50" s="48">
         <v>2000</v>
       </c>
@@ -9764,91 +9877,46 @@
         <f t="shared" si="10"/>
         <v>519.71329059303525</v>
       </c>
-      <c r="T50" s="90">
+      <c r="T50" s="66">
         <f t="shared" si="11"/>
         <v>0.21894138272331365</v>
       </c>
-      <c r="U50" s="74">
+      <c r="U50" s="64">
         <f t="shared" si="12"/>
         <v>0.22928201701963311</v>
       </c>
-      <c r="V50" s="77"/>
-      <c r="X50" s="96">
+      <c r="V50" s="89"/>
+      <c r="X50" s="71">
         <v>0.21894138272331365</v>
       </c>
-      <c r="Y50" s="97">
+      <c r="Y50" s="72">
         <v>0.22928201701963311</v>
       </c>
-      <c r="Z50" s="67"/>
+      <c r="Z50" s="88"/>
+      <c r="AA50" s="48">
+        <v>2000</v>
+      </c>
     </row>
-    <row r="51" spans="6:26" x14ac:dyDescent="0.3">
-      <c r="F51" s="87"/>
-      <c r="G51" s="89"/>
-      <c r="H51" s="89"/>
-      <c r="I51" s="89"/>
-      <c r="J51" s="89"/>
-      <c r="K51" s="89"/>
-      <c r="L51" s="89"/>
-      <c r="M51" s="89"/>
-      <c r="N51" s="89"/>
-      <c r="O51" s="89"/>
-      <c r="P51" s="89"/>
-      <c r="Q51" s="89"/>
-      <c r="R51" s="89"/>
-      <c r="S51" s="89"/>
-      <c r="T51" s="89"/>
-      <c r="U51" s="89"/>
+    <row r="51" spans="6:27" x14ac:dyDescent="0.3">
+      <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="6:26" x14ac:dyDescent="0.3">
-      <c r="F52" s="87"/>
-      <c r="G52" s="89"/>
-      <c r="H52" s="89"/>
-      <c r="I52" s="89"/>
-      <c r="J52" s="89"/>
-      <c r="K52" s="89"/>
-      <c r="L52" s="89"/>
-      <c r="M52" s="89"/>
-      <c r="N52" s="89"/>
-      <c r="O52" s="89"/>
-      <c r="P52" s="89"/>
-      <c r="Q52" s="89"/>
-      <c r="R52" s="89"/>
-      <c r="S52" s="89"/>
-      <c r="T52" s="89"/>
-      <c r="U52" s="89"/>
-    </row>
-    <row r="53" spans="6:26" x14ac:dyDescent="0.3">
-      <c r="F53" s="89"/>
-      <c r="G53" s="89"/>
-      <c r="H53" s="89"/>
-      <c r="I53" s="89"/>
-      <c r="J53" s="89"/>
-      <c r="K53" s="89"/>
-      <c r="L53" s="89"/>
-      <c r="M53" s="89"/>
-      <c r="N53" s="89"/>
-      <c r="O53" s="89"/>
-      <c r="P53" s="89"/>
-      <c r="Q53" s="89"/>
-      <c r="R53" s="89"/>
-      <c r="S53" s="89"/>
-      <c r="T53" s="89"/>
-      <c r="U53" s="89"/>
+    <row r="52" spans="6:27" x14ac:dyDescent="0.3">
+      <c r="F52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="V41:V50"/>
+    <mergeCell ref="Z41:Z50"/>
+    <mergeCell ref="V14:V27"/>
+    <mergeCell ref="V28:V40"/>
+    <mergeCell ref="Z3:Z13"/>
+    <mergeCell ref="Z14:Z27"/>
+    <mergeCell ref="Z28:Z40"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="V3:V13"/>
-    <mergeCell ref="V14:V27"/>
-    <mergeCell ref="V28:V40"/>
-    <mergeCell ref="Z3:Z13"/>
-    <mergeCell ref="Z14:Z27"/>
-    <mergeCell ref="Z28:Z40"/>
-    <mergeCell ref="V41:V50"/>
-    <mergeCell ref="Z41:Z50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>